<commit_message>
o zed só quer gaita
</commit_message>
<xml_diff>
--- a/UseCaseLI4.xlsx
+++ b/UseCaseLI4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\LI4\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6D2BF1-48F2-422B-B012-5017371DD0E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCB8375-D5DB-4E8A-B7A9-A17D0E7E759B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6984" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="136">
   <si>
     <t>Actor input</t>
   </si>
@@ -425,23 +425,10 @@
 </t>
   </si>
   <si>
-    <t>6. Receita é acrescentada ao sistema</t>
-  </si>
-  <si>
     <t xml:space="preserve">5. Valida cada um dos campos </t>
   </si>
   <si>
     <t>4. Preenche os campos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Apresenta campos necessários a 
-preencher de modo a poder adicionar
-a receita </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Verifica se a receita que se está a 
-tentar adicionar não se encontra já no
-sistema </t>
   </si>
   <si>
     <t>1. Solicita que pretende adicionar 
@@ -485,6 +472,28 @@
   </si>
   <si>
     <t>Alterar receita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception 2
+[Receita já existe] 
+Passo 2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Apresenta campos necessários a 
+preencher de modo a poder adicionar
+a receita </t>
+  </si>
+  <si>
+    <t>3. Preenche os campos</t>
+  </si>
+  <si>
+    <t>4. Verifica se a receita que se está a 
+tentar adicionar não se encontra já no
+sistema</t>
+  </si>
+  <si>
+    <t>5. Receita é acrescentada ao sistema</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1045,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1175,6 +1184,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1939,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDF3DAD-EB37-4EF0-AFA1-0482E8278584}">
-  <dimension ref="B1:D18"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1959,7 +1971,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D2" s="61"/>
     </row>
@@ -1968,7 +1980,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D3" s="61"/>
     </row>
@@ -1977,7 +1989,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D4" s="61"/>
     </row>
@@ -1986,7 +1998,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D5" s="63"/>
     </row>
@@ -2004,7 +2016,7 @@
     <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="65"/>
       <c r="C7" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2012,86 +2024,57 @@
       <c r="B8" s="65"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="65"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="65"/>
-      <c r="C10" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="1"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="82" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="65"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="65"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="81"/>
+      <c r="D12" s="12" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="59"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="80"/>
+    </row>
+    <row r="14" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="59"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="59"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="2:4" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="59"/>
-      <c r="C17" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="80"/>
-    </row>
-    <row r="18" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="59"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="78"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B13:B15"/>
+  <mergeCells count="6">
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2120,7 +2103,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D2" s="61"/>
     </row>
@@ -2129,7 +2112,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D3" s="61"/>
     </row>
@@ -2138,7 +2121,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D4" s="61"/>
     </row>
@@ -2147,7 +2130,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D5" s="63"/>
     </row>
@@ -2165,7 +2148,7 @@
     <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="65"/>
       <c r="C7" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2173,20 +2156,20 @@
       <c r="B8" s="65"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="55.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="65"/>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="65"/>
       <c r="C10" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2194,14 +2177,14 @@
       <c r="B11" s="65"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="65"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -2229,7 +2212,7 @@
       </c>
       <c r="C16" s="81"/>
       <c r="D16" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
o Johnny só fuma ganza marroquina
</commit_message>
<xml_diff>
--- a/UseCaseLI4.xlsx
+++ b/UseCaseLI4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\LI4\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCB8375-D5DB-4E8A-B7A9-A17D0E7E759B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BB8C15-4729-4963-AD50-18EA40A7965A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6984" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,10 +406,6 @@
     <t>2.2 Volta ao passo 1</t>
   </si>
   <si>
-    <t>2.1 Avisa que a receita que se pretende
-adicionar já se encontra no sistema</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comp Alt
 [Receita já existe] 
 Passo 2
@@ -474,12 +470,6 @@
     <t>Alterar receita</t>
   </si>
   <si>
-    <t xml:space="preserve">Exception 2
-[Receita já existe] 
-Passo 2
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">2. Apresenta campos necessários a 
 preencher de modo a poder adicionar
 a receita </t>
@@ -494,6 +484,16 @@
   </si>
   <si>
     <t>5. Receita é acrescentada ao sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception 1
+[Receita já existe] 
+Passo 4
+</t>
+  </si>
+  <si>
+    <t>4.1 Avisa que a receita que se pretende
+adicionar já se encontra no sistema</t>
   </si>
 </sst>
 </file>
@@ -1954,7 +1954,7 @@
   <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1971,7 +1971,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D2" s="61"/>
     </row>
@@ -1980,7 +1980,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" s="61"/>
     </row>
@@ -1989,7 +1989,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="61"/>
     </row>
@@ -1998,7 +1998,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="63"/>
     </row>
@@ -2016,7 +2016,7 @@
     <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="65"/>
       <c r="C7" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2024,13 +2024,13 @@
       <c r="B8" s="65"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="65"/>
       <c r="C9" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2038,23 +2038,23 @@
       <c r="B10" s="65"/>
       <c r="C10" s="5"/>
       <c r="D10" s="82" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="65"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="58" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C12" s="81"/>
       <c r="D12" s="12" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -2103,7 +2103,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="61"/>
     </row>
@@ -2112,7 +2112,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" s="61"/>
     </row>
@@ -2121,7 +2121,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="61"/>
     </row>
@@ -2130,7 +2130,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="63"/>
     </row>
@@ -2148,7 +2148,7 @@
     <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="65"/>
       <c r="C7" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2156,20 +2156,20 @@
       <c r="B8" s="65"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="55.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="65"/>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="65"/>
       <c r="C10" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2177,23 +2177,23 @@
       <c r="B11" s="65"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="65"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -2208,11 +2208,11 @@
     </row>
     <row r="16" spans="2:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="81"/>
       <c r="D16" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
o zed até chupa bem xD
</commit_message>
<xml_diff>
--- a/UseCaseLI4.xlsx
+++ b/UseCaseLI4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaon\Desktop\LI4\Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\LI4\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59F89F5-9C38-47B0-B021-069B6C35AD7C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E15086-F519-453A-8DBB-3387047C5FB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registar conta" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,13 @@
     <sheet name="Visualizar todas as receitas " sheetId="10" r:id="rId5"/>
     <sheet name="Alterar dados pessoais" sheetId="4" r:id="rId6"/>
     <sheet name="Gerir preferências" sheetId="6" r:id="rId7"/>
-    <sheet name="Pedir histórico" sheetId="22" r:id="rId8"/>
-    <sheet name="Consultar dificuldades " sheetId="24" r:id="rId9"/>
-    <sheet name="Solicitar uma ementa semanal" sheetId="17" r:id="rId10"/>
-    <sheet name="Lista ingredientes semanal" sheetId="8" r:id="rId11"/>
-    <sheet name="Realizar uma receita" sheetId="15" r:id="rId12"/>
+    <sheet name="Solicitar uma ementa semanal" sheetId="17" r:id="rId8"/>
+    <sheet name="Lista ingredientes semanal" sheetId="8" r:id="rId9"/>
+    <sheet name="Realizar uma receita" sheetId="15" r:id="rId10"/>
+    <sheet name="Adicionar receita" sheetId="20" r:id="rId11"/>
+    <sheet name="Alterar receita" sheetId="21" r:id="rId12"/>
+    <sheet name="Pedir histórico" sheetId="22" r:id="rId13"/>
+    <sheet name="Consultar dificuldades " sheetId="23" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="147">
   <si>
     <t>Actor input</t>
   </si>
@@ -201,9 +203,6 @@
   </si>
   <si>
     <t>2. Confirma que tem os ingredientes necessários e avança</t>
-  </si>
-  <si>
-    <t>1. Apresenta ingredientes necessários para a confeção do  prato</t>
   </si>
   <si>
     <t>Cliente autenticado &amp;&amp; receita a realizar selecionada &amp;&amp; utensílios necessários</t>
@@ -315,9 +314,6 @@
   </si>
   <si>
     <t>3.2. Pergunta ao utilizador se pretende continuar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1.Informa sobre a impossivel de não repetir receitas </t>
   </si>
   <si>
     <t>Alternativa 1 (Passo 2)
@@ -403,38 +399,115 @@
 (passo 3)</t>
   </si>
   <si>
-    <t>Pedir histórico</t>
-  </si>
-  <si>
-    <t>Apresenta lista com pratos confecionados e dificuldades encontradas</t>
+    <t xml:space="preserve">3.1.Informa sobre a impossibilidade de não repetir receitas </t>
+  </si>
+  <si>
+    <t>5.1 Avisa acerca dos campos inválidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Valida cada um dos campos </t>
+  </si>
+  <si>
+    <t>4. Preenche os campos</t>
+  </si>
+  <si>
+    <t>1. Solicita que pretende adicionar 
+uma receita</t>
+  </si>
+  <si>
+    <t>Receita é adicionada ao sistema</t>
+  </si>
+  <si>
+    <t>Admin está autenticado</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Adicionar receita</t>
+  </si>
+  <si>
+    <t>6. Receita é alterada no sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Apresenta campos necessários a 
+preencher de modo a poder alterar
+a receita </t>
+  </si>
+  <si>
+    <t>2. Verifica se a receita que se pretende 
+alterar existe no sistema</t>
+  </si>
+  <si>
+    <t>1. Solicita que pretende alterar 
+uma receita</t>
+  </si>
+  <si>
+    <t>Receita é alterada</t>
+  </si>
+  <si>
+    <t>Alterar receita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Apresenta campos necessários a 
+preencher de modo a poder adicionar
+a receita </t>
+  </si>
+  <si>
+    <t>3. Preenche os campos</t>
+  </si>
+  <si>
+    <t>4. Verifica se a receita que se está a 
+tentar adicionar não se encontra já no
+sistema</t>
+  </si>
+  <si>
+    <t>5. Receita é acrescentada ao sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception 1
+[Receita já existe] 
+Passo 4
+</t>
+  </si>
+  <si>
+    <t>4.1 Avisa que a receita que se pretende
+adicionar já se encontra no sistema</t>
+  </si>
+  <si>
+    <t>2.1 Avisa que a receita que se pretende
+alterar não se encontra no sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception 1
+[Campos Inválidos] 
+Passo 5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception 2
+[Receita não existe] 
+Passo 2
+</t>
+  </si>
+  <si>
+    <t>1. Apresenta ingredientes e utensílios necessários para a confeção do  prato</t>
+  </si>
+  <si>
+    <t>2. Carrega e apresenta o histórico ao cliente</t>
   </si>
   <si>
     <t>1. Solicita para apresentar o seu 
 histórico</t>
   </si>
   <si>
-    <t>2. Carrega e apresenta o histórico ao cliente</t>
-  </si>
-  <si>
-    <t>Consultar dificuldades encontradas</t>
-  </si>
-  <si>
-    <t>Cliente autenticado &amp;&amp; histórico estar apresentado</t>
-  </si>
-  <si>
-    <t>Apresenta dificuldade encontrada para dada receita confecionada</t>
-  </si>
-  <si>
-    <t>1. Seleciona uma receita da lista 
-de receitas confecionadas</t>
-  </si>
-  <si>
-    <t>2. Carrega as dificuldades encontradas do cliente
-na dada receita</t>
-  </si>
-  <si>
-    <t>3. Mostra as dificuldades encontradas ao 
-cliente</t>
+    <t>Apresenta lista com pratos confecionados e dificuldades encontradas</t>
+  </si>
+  <si>
+    <t>Pedir histórico</t>
+  </si>
+  <si>
+    <t>2.1 Avisa da impossibilidade de mostrar a dificuldades encontradas na dada receita</t>
   </si>
   <si>
     <t xml:space="preserve">Exception 1
@@ -443,7 +516,25 @@
 </t>
   </si>
   <si>
-    <t>2.1 Avisa da impossibilidade de mostrar a dificuldades encontradas na dada receita</t>
+    <t>3. Mostra as dificuldades encontradas ao 
+cliente</t>
+  </si>
+  <si>
+    <t>2. Carrega as dificuldades encontradas do cliente
+da dada receita</t>
+  </si>
+  <si>
+    <t>1. Seleciona uma receita da lista 
+de receitas confecionadas</t>
+  </si>
+  <si>
+    <t>Apresenta dificuldade encontrada para dada receita confecionada</t>
+  </si>
+  <si>
+    <t>Cliente autenticado &amp;&amp; histórico estar apresentado</t>
+  </si>
+  <si>
+    <t>Consultar dificuldades encontradas</t>
   </si>
 </sst>
 </file>
@@ -501,7 +592,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,13 +607,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1001,7 +1086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1051,7 +1136,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1065,7 +1149,14 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1111,12 +1202,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1126,14 +1211,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1468,38 +1546,38 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="47"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="54" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1510,75 +1588,75 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="51"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="55"/>
+      <c r="C8" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="51"/>
-      <c r="C8" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="51"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="10"/>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="51"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="51"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="5"/>
       <c r="D11" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="44" t="s">
-        <v>68</v>
+      <c r="B12" s="48" t="s">
+        <v>67</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="45"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="45"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="44" t="s">
-        <v>69</v>
+      <c r="B15" s="48" t="s">
+        <v>68</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="45"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="45"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
@@ -1597,378 +1675,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5" style="17" customWidth="1"/>
-    <col min="2" max="2" width="16.09765625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="33.3984375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="72.5" style="17" customWidth="1"/>
-    <col min="5" max="256" width="10.8984375" style="17" customWidth="1"/>
-    <col min="257" max="16384" width="10.8984375" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="32"/>
-    </row>
-    <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="21"/>
-      <c r="B2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="21"/>
-      <c r="B3" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="18"/>
-    </row>
-    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="21"/>
-      <c r="B4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="21"/>
-      <c r="B5" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="21"/>
-      <c r="B6" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="21"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="21"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5" ht="45.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="21"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="21"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="21"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="1:5" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="21"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="21"/>
-      <c r="B17" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="18"/>
-    </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="21"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="18"/>
-    </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="21"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="18"/>
-    </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="21"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="21"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="1:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="21"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="18"/>
-    </row>
-    <row r="23" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="24"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="60"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="22"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="60"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="34"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="60"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="34"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="60"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="34"/>
-    </row>
-    <row r="28" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="60"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B22"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.19921875" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="47"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="47"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="47"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="51"/>
-      <c r="C7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="51"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="51"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1984,40 +1695,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="47"/>
+      <c r="C4" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="49"/>
+      <c r="C5" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2028,69 +1739,69 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="63"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="63"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="63"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="63"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="63"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="63"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="63"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="63"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="63"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="63"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="48" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="4"/>
@@ -2099,26 +1810,26 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="44"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="45"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="45"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="45"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>42</v>
@@ -2126,13 +1837,13 @@
       <c r="G21" s="15"/>
     </row>
     <row r="22" spans="2:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="45"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="6"/>
       <c r="D22" s="3"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="48" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -2141,36 +1852,36 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="44"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="5"/>
       <c r="D24" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="45"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="45"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="45"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="5"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="45"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="6"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="48" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -2179,40 +1890,40 @@
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="44"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="5"/>
       <c r="D30" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="45"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="5"/>
       <c r="D31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="45"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="16"/>
       <c r="D32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="45"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="45"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="6"/>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="48" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="4"/>
@@ -2221,28 +1932,28 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="44"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="5"/>
       <c r="D36" s="1"/>
       <c r="F36" s="15"/>
     </row>
     <row r="37" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="45"/>
+      <c r="B37" s="49"/>
       <c r="C37" s="5"/>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="45"/>
+      <c r="B38" s="49"/>
       <c r="C38" s="5"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="45"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="5"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="45"/>
+      <c r="B40" s="49"/>
       <c r="C40" s="6"/>
       <c r="D40" s="3"/>
     </row>
@@ -2263,12 +1974,519 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDF3DAD-EB37-4EF0-AFA1-0482E8278584}">
+  <dimension ref="B1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" customWidth="1"/>
+    <col min="3" max="3" width="33.296875" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="51"/>
+    </row>
+    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="51"/>
+    </row>
+    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="51"/>
+    </row>
+    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="53"/>
+    </row>
+    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="55"/>
+      <c r="C7" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="55"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="55"/>
+      <c r="C9" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="55"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="55"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="46"/>
+      <c r="D12" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="49"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="45"/>
+    </row>
+    <row r="14" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="49"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AC8AF1-4945-4E90-9CFB-2C6E3F0B0D9F}">
+  <dimension ref="B1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" customWidth="1"/>
+    <col min="3" max="3" width="33.296875" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="51"/>
+    </row>
+    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="51"/>
+    </row>
+    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="51"/>
+    </row>
+    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="53"/>
+    </row>
+    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="55"/>
+      <c r="C7" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="55"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="55.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="55"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="55"/>
+      <c r="C10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="55"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="55"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="49"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="49"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="46"/>
+      <c r="D16" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="49"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="45"/>
+    </row>
+    <row r="18" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="49"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B13:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F73DAE4-4797-4ED3-85CB-1452BD9F6405}">
+  <dimension ref="B1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="33.19921875" customWidth="1"/>
+    <col min="4" max="4" width="46.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="51"/>
+    </row>
+    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="51"/>
+    </row>
+    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="51"/>
+    </row>
+    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="53"/>
+    </row>
+    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="55"/>
+      <c r="C7" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="55"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C7ADAA-F745-434B-8977-383BAFA1EFD9}">
+  <dimension ref="B1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="33.19921875" customWidth="1"/>
+    <col min="4" max="4" width="46.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="51"/>
+    </row>
+    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="51"/>
+    </row>
+    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="51"/>
+    </row>
+    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="53"/>
+    </row>
+    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="55"/>
+      <c r="C7" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="55"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="47" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="55"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="46"/>
+      <c r="D10" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="55"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="45"/>
+    </row>
+    <row r="12" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="55"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="45"/>
+    </row>
+    <row r="13" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="55"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2282,59 +2500,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="55"/>
+      <c r="C2" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="59"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21"/>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="55"/>
+      <c r="C3" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="59"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="21"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="55"/>
+      <c r="C4" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="59"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="21"/>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="53"/>
+      <c r="C5" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="57"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="60" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2347,101 +2565,101 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="57"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="57"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="23"/>
       <c r="D8" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="57"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="23"/>
       <c r="D9" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="57"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="57"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="57"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
-      <c r="B13" s="57"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="21"/>
-      <c r="B14" s="57"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="23"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="21"/>
-      <c r="B15" s="57"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="21"/>
-      <c r="B16" s="57"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="20"/>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
-      <c r="B17" s="56" t="s">
-        <v>55</v>
+      <c r="B17" s="60" t="s">
+        <v>54</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
-      <c r="B18" s="57"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="23"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
-      <c r="B19" s="57"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="20"/>
       <c r="D19" s="19"/>
       <c r="E19" s="18"/>
@@ -2468,7 +2686,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2482,59 +2700,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="55"/>
+      <c r="C2" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="59"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21"/>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="21"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="21"/>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="53"/>
+      <c r="C5" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="57"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="60" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2547,104 +2765,104 @@
     </row>
     <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="40"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="39"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="39"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="57"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="57"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="57"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="57"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
-      <c r="B13" s="57"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
-      <c r="B14" s="57"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="23"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
-      <c r="B15" s="57"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
-      <c r="B16" s="57"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="20"/>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
-      <c r="B17" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>95</v>
+      <c r="B17" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>93</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
-      <c r="B18" s="58"/>
+      <c r="B18" s="62"/>
       <c r="C18" s="23"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="19"/>
       <c r="E19" s="18"/>
     </row>
@@ -2684,59 +2902,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="55"/>
+      <c r="C2" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="59"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21"/>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="21"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="21"/>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="53"/>
+      <c r="C5" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="57"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="60" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2749,68 +2967,68 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="40" t="s">
-        <v>108</v>
+      <c r="B7" s="61"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="39" t="s">
+        <v>106</v>
       </c>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="39"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="60"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="36" t="s">
-        <v>106</v>
+      <c r="D9" s="35" t="s">
+        <v>104</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="60"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="60"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="42" t="s">
-        <v>103</v>
+      <c r="B12" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="41" t="s">
+        <v>101</v>
       </c>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
-      <c r="B13" s="60"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="21"/>
-      <c r="B14" s="60"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="20"/>
       <c r="D14" s="19"/>
       <c r="E14" s="18"/>
@@ -2853,40 +3071,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="54" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2897,14 +3115,14 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="51"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="51"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="6"/>
       <c r="D8" s="14" t="s">
         <v>28</v>
@@ -2946,40 +3164,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="54" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2990,49 +3208,49 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="51"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="55"/>
+      <c r="C8" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="51"/>
-      <c r="C8" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="51"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="51"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="5"/>
       <c r="D10" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="44" t="s">
-        <v>76</v>
+      <c r="B11" s="48" t="s">
+        <v>75</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="45"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="45"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
@@ -3073,40 +3291,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="54" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3117,49 +3335,49 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="51"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="51"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="51"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="51"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="44" t="s">
-        <v>111</v>
+      <c r="B11" s="48" t="s">
+        <v>109</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="45"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="45"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
@@ -3180,11 +3398,275 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5A95F6-4F65-4770-AD33-698E04AE30DA}">
-  <dimension ref="B1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.09765625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="33.3984375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="72.5" style="17" customWidth="1"/>
+    <col min="5" max="256" width="10.8984375" style="17" customWidth="1"/>
+    <col min="257" max="16384" width="10.8984375" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="21"/>
+      <c r="B2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21"/>
+      <c r="B3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="59"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="21"/>
+      <c r="B4" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="59"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="21"/>
+      <c r="B5" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="57"/>
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="21"/>
+      <c r="B6" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="21"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="21"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" ht="45.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="21"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="21"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="21"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" spans="1:5" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="21"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="21"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="21"/>
+      <c r="B17" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="21"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="21"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="21"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="21"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="21"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="61"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="61"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="33"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="61"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="33"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="61"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="33"/>
+    </row>
+    <row r="28" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="61"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="B17:B22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3192,7 +3674,7 @@
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.19921875" customWidth="1"/>
     <col min="3" max="3" width="33.19921875" customWidth="1"/>
-    <col min="4" max="4" width="46.5" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -3200,40 +3682,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="47"/>
+      <c r="C2" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="47"/>
+      <c r="C4" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="49"/>
+      <c r="C5" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="54" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3244,146 +3726,33 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="51"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="10" t="s">
-        <v>114</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="51"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:4" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="55"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="55"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C610B27-4ECF-4388-B5CD-61356E9DF7A4}">
-  <dimension ref="B1:D13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.19921875" customWidth="1"/>
-    <col min="4" max="4" width="46.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="47"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="47"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="47"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="51"/>
-      <c r="C7" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="51"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="64" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="51"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="51"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="65"/>
-    </row>
-    <row r="12" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="51"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="65"/>
-    </row>
-    <row r="13" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="51"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="66"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>

<commit_message>
excel atualizado, realizar receita
</commit_message>
<xml_diff>
--- a/UseCaseLI4.xlsx
+++ b/UseCaseLI4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaon\Desktop\LI4\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11F0B2B-C33A-42D6-A8DB-7B89D1464C10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2113B801-B065-4A5A-9027-220742BCC0DD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registar conta" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="151">
   <si>
     <t>Actor input</t>
   </si>
@@ -138,68 +138,11 @@
     <t>Realizar uma receita</t>
   </si>
   <si>
-    <t>6.1. Volta ao passo 4</t>
-  </si>
-  <si>
-    <t>Cenário Alt 3
-[Existem mais passos a realizar]     (passo 6)</t>
-  </si>
-  <si>
-    <t>5.2.5. Volta ao passo 5</t>
-  </si>
-  <si>
-    <t>5.2.4. Guarda no histórico a dúvida relativa a este passo</t>
-  </si>
-  <si>
-    <t>5.2.3. Apresenta um vídeo ou imagem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.2.2. Interpreta a dúvida </t>
-  </si>
-  <si>
-    <t>5.2.1. Avisa o sistema sobre a dúvida</t>
-  </si>
-  <si>
-    <t>Cenário Alt 2
-[O cliente tem dúvidas sobre    o passo]     (passo 5)</t>
-  </si>
-  <si>
-    <t>5.1.3. Volta ao passo 5</t>
-  </si>
-  <si>
-    <t>5.1.1. Pede para repetir o passo</t>
-  </si>
-  <si>
-    <t>Cenário Alt 1
-[O cliente não percebeu, de todo o passo]     (passo 5)</t>
-  </si>
-  <si>
-    <t>2.4. Apresenta os locais mais próximos ao utilizador</t>
-  </si>
-  <si>
-    <t>2.3. Calcula os locais mais próximos para comprar os ingredientes</t>
-  </si>
-  <si>
-    <t>2.2. Indica, por voz ou escrita, os ingredientes em falta.</t>
-  </si>
-  <si>
     <t>2.1. Pergunta quais o ingredientes em falta</t>
   </si>
   <si>
     <t>Cenário Exec. 1
 [O cliente não possuí os ingredientes necessários]     (passo 2)</t>
-  </si>
-  <si>
-    <t>6. Verifica que não existem mais passos.</t>
-  </si>
-  <si>
-    <t>5.Percebe e confirma que pode avançar para o próximo passo por voz ou escrita</t>
-  </si>
-  <si>
-    <t>4. Lê o próximo passo a efetuar</t>
-  </si>
-  <si>
-    <t>3. Apresenta a lista de passos</t>
   </si>
   <si>
     <t>2. Confirma que tem os ingredientes necessários e avança</t>
@@ -295,9 +238,6 @@
   </si>
   <si>
     <t>Receita realizada &amp;&amp; Realização da receita guardada no histórico</t>
-  </si>
-  <si>
-    <t>5.1.2. Repete a leitura do passo</t>
   </si>
   <si>
     <t>3.3.1. Diz que não</t>
@@ -537,6 +477,82 @@
   </si>
   <si>
     <t>2. Carrega e apresenta o histórico de refeições ao cliente</t>
+  </si>
+  <si>
+    <t>3. Começa a contagem de tempo de confeção da receita</t>
+  </si>
+  <si>
+    <t>4. Apresenta a lista de passos</t>
+  </si>
+  <si>
+    <t>5. Lê o próximo passo a efetuar</t>
+  </si>
+  <si>
+    <t>6. Percebe e confirma que pode avançar para o próximo passo por voz ou escrita</t>
+  </si>
+  <si>
+    <t>7. Verifica que não existem mais passos</t>
+  </si>
+  <si>
+    <t>Cenário Alt 1
+[O cliente não percebeu, de todo o passo]     (passo 6)</t>
+  </si>
+  <si>
+    <t>Cenário Alt 2
+[O cliente tem dúvidas sobre    o passo]     (passo 6)</t>
+  </si>
+  <si>
+    <t>Cenário Alt 3
+[Existem mais passos a realizar]     (passo 7)</t>
+  </si>
+  <si>
+    <t>6.1.1. Pede para repetir o passo</t>
+  </si>
+  <si>
+    <t>6.1.2. Repete a leitura do passo</t>
+  </si>
+  <si>
+    <t>6.1.3. Volta ao passo 5</t>
+  </si>
+  <si>
+    <t>6.2.1. Avisa o sistema sobre a dúvida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.2.2. Interpreta a dúvida </t>
+  </si>
+  <si>
+    <t>6.2.3. Apresenta um vídeo ou imagem</t>
+  </si>
+  <si>
+    <t>6.2.4. Guarda no histórico a dúvida relativa a este passo</t>
+  </si>
+  <si>
+    <t>6.2.5. Volta ao passo 5</t>
+  </si>
+  <si>
+    <t>7.1. Volta ao passo 4</t>
+  </si>
+  <si>
+    <t>Cenário Exec. 2
+[Impossível 
+consultar 
+localização
+atual]
+(passo 2.3)</t>
+  </si>
+  <si>
+    <t>2.3.1 Sistema informa da impossibilidade de calcular a localização atual 
+do cliente</t>
+  </si>
+  <si>
+    <t>2.2. Indica, por voz ou escrita, os ingredientes em falta</t>
+  </si>
+  <si>
+    <t>2.3. Calcula os locais mais próximos para comprar os ingredientes, consoante 
+a localização atual do cliente</t>
+  </si>
+  <si>
+    <t>2.4. Apresenta os locais mais próximos ao utilizador</t>
   </si>
 </sst>
 </file>
@@ -614,7 +630,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1083,12 +1099,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1160,6 +1209,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1208,15 +1260,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1551,38 +1607,38 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1593,75 +1649,75 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="5" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="10"/>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="5"/>
       <c r="D11" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="49" t="s">
-        <v>67</v>
+      <c r="B12" s="50" t="s">
+        <v>49</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="50"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="50"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="49" t="s">
-        <v>68</v>
+      <c r="B15" s="50" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="50"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="50"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
@@ -1681,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="B1:G40"/>
+  <dimension ref="B1:G41"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1700,40 +1756,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="52"/>
+      <c r="C4" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="68" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1744,235 +1800,250 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="66"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="66"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="66"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="66"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="66"/>
-      <c r="C11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="1"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="66"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="66"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="66"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="66"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
+      <c r="B15" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="66"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2" t="s">
-        <v>45</v>
+      <c r="B16" s="50"/>
+      <c r="C16" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="51"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="11" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="49"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="50"/>
-      <c r="C19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="50"/>
+      <c r="D18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="2:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="51"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="2:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="66" t="s">
+        <v>146</v>
+      </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="50"/>
+      <c r="D20" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="67"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="2:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="50"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="3"/>
+    <row r="22" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="67"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="49"/>
+    <row r="23" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="67"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="2:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="67"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="D24" s="1"/>
+      <c r="G24" s="15"/>
     </row>
     <row r="25" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="50"/>
-      <c r="C25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="1"/>
+      <c r="B25" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="50"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="27" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="50"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="50"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="3"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="2"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="49"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="B30" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="50"/>
       <c r="C31" s="5"/>
       <c r="D31" s="1" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="50"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="50"/>
-      <c r="C33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="1"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="34" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="50"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="3"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="1"/>
     </row>
     <row r="35" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="B35" s="51"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="49"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="1"/>
-      <c r="F36" s="15"/>
+      <c r="B36" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="37" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="50"/>
       <c r="C37" s="5"/>
       <c r="D37" s="1"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="50"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="5"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="50"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="5"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="50"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D41" s="70"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="B17:B22"/>
+  <mergeCells count="10">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B15:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2000,40 +2071,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="52"/>
+      <c r="C2" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="52"/>
+      <c r="C3" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="52"/>
+      <c r="C4" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2044,59 +2115,59 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:6" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="5" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:6" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="5"/>
       <c r="D10" s="47" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="49" t="s">
-        <v>129</v>
+      <c r="B12" s="50" t="s">
+        <v>110</v>
       </c>
       <c r="C12" s="46"/>
       <c r="D12" s="12" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="50"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="5"/>
       <c r="D13" s="45"/>
     </row>
     <row r="14" spans="2:6" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="50"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="44"/>
       <c r="D14" s="43"/>
     </row>
@@ -2135,40 +2206,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="52"/>
+      <c r="C2" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="52"/>
+      <c r="C3" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="52"/>
+      <c r="C4" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2179,82 +2250,82 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="55.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="5" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="56"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="49" t="s">
-        <v>132</v>
+      <c r="B13" s="50" t="s">
+        <v>113</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="50"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="50"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="2:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="49" t="s">
-        <v>133</v>
+      <c r="B16" s="50" t="s">
+        <v>114</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="12" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="50"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="5"/>
       <c r="D17" s="45"/>
     </row>
     <row r="18" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="50"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="44"/>
       <c r="D18" s="43"/>
     </row>
@@ -2294,40 +2365,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="52"/>
+      <c r="C2" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2338,17 +2409,17 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="67" t="s">
-        <v>146</v>
+      <c r="D7" s="49" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2370,7 +2441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C7ADAA-F745-434B-8977-383BAFA1EFD9}">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -2387,40 +2458,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="52"/>
+      <c r="C2" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="52"/>
+      <c r="C4" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="54"/>
+      <c r="C5" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2431,47 +2502,47 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="10"/>
       <c r="D8" s="47" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="55" t="s">
-        <v>138</v>
+      <c r="B10" s="56" t="s">
+        <v>119</v>
       </c>
       <c r="C10" s="46"/>
       <c r="D10" s="12" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="48"/>
       <c r="D11" s="45"/>
     </row>
     <row r="12" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="56"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="48"/>
       <c r="D12" s="45"/>
     </row>
     <row r="13" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="44"/>
       <c r="D13" s="43"/>
     </row>
@@ -2519,10 +2590,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="60"/>
+      <c r="C2" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="61"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2530,10 +2601,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="60"/>
+      <c r="C3" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="61"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2541,10 +2612,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="60"/>
+      <c r="C4" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="61"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2552,15 +2623,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="58"/>
+      <c r="C5" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="59"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="62" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2573,59 +2644,59 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="62"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="28" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="62"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="23"/>
       <c r="D8" s="26" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="62"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="23"/>
       <c r="D9" s="26" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="62"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="61" t="s">
-        <v>54</v>
+      <c r="B11" s="62" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="24" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="62"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
-      <c r="B13" s="62"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="20"/>
       <c r="D13" s="19"/>
       <c r="E13" s="18"/>
@@ -2677,10 +2748,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="60"/>
+      <c r="C2" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="61"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2688,10 +2759,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2699,10 +2770,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2710,15 +2781,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="58"/>
+      <c r="C5" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="59"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="62" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2731,103 +2802,103 @@
     </row>
     <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="62"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="40" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="62"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="62"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="23" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="62"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="62"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="62"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
-      <c r="B13" s="62"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
-      <c r="B14" s="62"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="23"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
-      <c r="B15" s="62"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
-      <c r="B16" s="62"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="20"/>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
-      <c r="B17" s="61" t="s">
-        <v>94</v>
+      <c r="B17" s="62" t="s">
+        <v>75</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
-      <c r="B18" s="63"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="23"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
-      <c r="B19" s="63"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="36"/>
       <c r="D19" s="19"/>
       <c r="E19" s="18"/>
@@ -2879,10 +2950,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="60"/>
+      <c r="C2" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="61"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2890,10 +2961,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2901,10 +2972,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2912,15 +2983,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="58"/>
+      <c r="C5" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="59"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="62" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2933,68 +3004,68 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="62"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="40"/>
       <c r="D7" s="39" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="62"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="62"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="23"/>
       <c r="D9" s="35" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="62"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="23" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="62"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="61" t="s">
-        <v>102</v>
+      <c r="B12" s="62" t="s">
+        <v>83</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="41" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
-      <c r="B13" s="62"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="21"/>
-      <c r="B14" s="62"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="20"/>
       <c r="D14" s="19"/>
       <c r="E14" s="18"/>
@@ -3021,7 +3092,7 @@
   <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3037,40 +3108,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3081,14 +3152,14 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="6"/>
       <c r="D8" s="14" t="s">
         <v>28</v>
@@ -3130,40 +3201,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3174,49 +3245,49 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="5" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="5"/>
       <c r="D10" s="11" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="49" t="s">
-        <v>75</v>
+      <c r="B11" s="50" t="s">
+        <v>57</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="50"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="50"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
@@ -3257,40 +3328,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3301,49 +3372,49 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="49" t="s">
-        <v>109</v>
+      <c r="B11" s="50" t="s">
+        <v>90</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="12" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="50"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="50"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
@@ -3393,10 +3464,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="60"/>
+      <c r="C2" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="61"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3404,10 +3475,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3415,10 +3486,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="60"/>
+      <c r="C4" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="61"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3426,15 +3497,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="58"/>
+      <c r="C5" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="59"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="62" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -3447,165 +3518,165 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="62"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="28" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="62"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="23"/>
       <c r="D8" s="35" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="45.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="62"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="23"/>
       <c r="D9" s="35" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="62"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="62"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="62"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
-      <c r="B13" s="62"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
-      <c r="B14" s="62"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="23"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
-      <c r="B15" s="62"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
-      <c r="B16" s="62"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="20"/>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
-      <c r="B17" s="61" t="s">
-        <v>85</v>
+      <c r="B17" s="62" t="s">
+        <v>66</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="24" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
-      <c r="B18" s="62"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="23"/>
       <c r="D18" s="22" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
-      <c r="B19" s="62"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="34" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="21"/>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="34"/>
       <c r="D20" s="33" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="21"/>
-      <c r="B21" s="62"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="34"/>
       <c r="D21" s="33"/>
       <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="21"/>
-      <c r="B22" s="62"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="20"/>
       <c r="D22" s="19"/>
       <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="61" t="s">
-        <v>81</v>
+      <c r="B23" s="62" t="s">
+        <v>62</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="62"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="23"/>
       <c r="D24" s="22"/>
     </row>
     <row r="25" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="62"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="34"/>
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="62"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="34"/>
       <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="62"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="34"/>
       <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="62"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="20"/>
       <c r="D28" s="19"/>
     </row>
@@ -3632,7 +3703,7 @@
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3648,40 +3719,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="52"/>
+      <c r="C4" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3692,21 +3763,21 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Excel atualizado consultar detalhes receita
</commit_message>
<xml_diff>
--- a/UseCaseLI4.xlsx
+++ b/UseCaseLI4.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaon\Desktop\LI4\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2113B801-B065-4A5A-9027-220742BCC0DD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854AD0B2-9788-40E4-A2CE-164AE3115D21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registar conta" sheetId="1" r:id="rId1"/>
     <sheet name="Fazer Login" sheetId="16" r:id="rId2"/>
     <sheet name="Desativar conta" sheetId="18" r:id="rId3"/>
-    <sheet name="Escolher receita pref" sheetId="19" r:id="rId4"/>
+    <sheet name="Solicitar receita pref" sheetId="19" r:id="rId4"/>
     <sheet name="Visualizar todas as receitas " sheetId="10" r:id="rId5"/>
     <sheet name="Alterar dados pessoais" sheetId="4" r:id="rId6"/>
     <sheet name="Gerir preferências" sheetId="6" r:id="rId7"/>
@@ -26,7 +26,7 @@
     <sheet name="Adicionar receita" sheetId="20" r:id="rId11"/>
     <sheet name="Alterar receita" sheetId="21" r:id="rId12"/>
     <sheet name="Pedir histórico" sheetId="22" r:id="rId13"/>
-    <sheet name="Consultar dificuldades " sheetId="23" r:id="rId14"/>
+    <sheet name="Consultar detalhes historico " sheetId="23" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="150">
   <si>
     <t>Actor input</t>
   </si>
@@ -86,9 +86,6 @@
   <si>
     <t>2. Seleciona os ingredientes que 
 não aprecia</t>
-  </si>
-  <si>
-    <t>Visualizar lista de ingredientes semanal</t>
   </si>
   <si>
     <t xml:space="preserve">Lista de ingredientes semanal é apresentada </t>
@@ -331,9 +328,6 @@
     <t>Receita escolhida com sucesso</t>
   </si>
   <si>
-    <t>Escolher receita com base nas suas preferências</t>
-  </si>
-  <si>
     <t>Exception 1
 [Preferências ambíguas] 
 (passo 3)</t>
@@ -440,34 +434,11 @@
     <t>Pedir histórico</t>
   </si>
   <si>
-    <t>2.1 Avisa da impossibilidade de mostrar a dificuldades encontradas na dada receita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exception 1
-[Não há dificuldades] 
-(passo 2)
-</t>
-  </si>
-  <si>
-    <t>3. Mostra as dificuldades encontradas ao 
-cliente</t>
-  </si>
-  <si>
-    <t>2. Carrega as dificuldades encontradas do cliente
-da dada receita</t>
-  </si>
-  <si>
     <t>1. Seleciona uma receita da lista 
 de receitas confecionadas</t>
   </si>
   <si>
-    <t>Apresenta dificuldade encontrada para dada receita confecionada</t>
-  </si>
-  <si>
     <t>Cliente autenticado &amp;&amp; histórico estar apresentado</t>
-  </si>
-  <si>
-    <t>Consultar dificuldades encontradas</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -553,6 +524,28 @@
   </si>
   <si>
     <t>2.4. Apresenta os locais mais próximos ao utilizador</t>
+  </si>
+  <si>
+    <t>Consultar detalhes de uma receita no histórico</t>
+  </si>
+  <si>
+    <t>Apresenta detalhes para dada receita confecionada</t>
+  </si>
+  <si>
+    <t>3. Carrega as dificuldades que o cliente encontrou ao confecionar a receita selecionada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Mostra ao cliente os detalhes da receita 
+</t>
+  </si>
+  <si>
+    <t>2. Carrega os dados da dada receita selecionada</t>
+  </si>
+  <si>
+    <t>Solicitar receita com base nas suas preferências</t>
+  </si>
+  <si>
+    <t>Visualizar lista de ingredientes da ementa semanal</t>
   </si>
 </sst>
 </file>
@@ -630,7 +623,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1132,12 +1125,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1208,9 +1225,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1272,7 +1295,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1591,7 +1616,7 @@
   <dimension ref="B1:D17"/>
   <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1607,38 +1632,38 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="53"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="53"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="55"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1649,75 +1674,75 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="59"/>
+      <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
-      <c r="C8" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="57"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="10"/>
       <c r="D9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="57"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="57"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="50" t="s">
-        <v>49</v>
+      <c r="B12" s="52" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="51"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="51"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="50" t="s">
-        <v>50</v>
+      <c r="B15" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="51"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="51"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
@@ -1739,7 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -1756,40 +1781,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="70" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1800,237 +1825,237 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="69"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="69"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="69"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="69"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="69"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="69"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="69"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="69"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="50" t="s">
-        <v>32</v>
+      <c r="B15" s="52" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="50"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:7" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="51"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="5"/>
       <c r="D17" s="11" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="51"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G18" s="15"/>
     </row>
     <row r="19" spans="2:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="51"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
       <c r="G19" s="15"/>
     </row>
     <row r="20" spans="2:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="66" t="s">
-        <v>146</v>
+      <c r="B20" s="68" t="s">
+        <v>138</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="11" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="67"/>
+      <c r="B21" s="69"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1"/>
       <c r="G21" s="15"/>
     </row>
     <row r="22" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="67"/>
+      <c r="B22" s="69"/>
       <c r="C22" s="5"/>
       <c r="D22" s="1"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="67"/>
+      <c r="B23" s="69"/>
       <c r="C23" s="5"/>
       <c r="D23" s="1"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" spans="2:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="67"/>
+      <c r="B24" s="69"/>
       <c r="C24" s="5"/>
       <c r="D24" s="1"/>
       <c r="G24" s="15"/>
     </row>
     <row r="25" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="50" t="s">
-        <v>134</v>
+      <c r="B25" s="52" t="s">
+        <v>126</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="50"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="51"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="5" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="51"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="5"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="51"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="5"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="50" t="s">
-        <v>135</v>
+      <c r="B30" s="52" t="s">
+        <v>127</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="50"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="5"/>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="51"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="51"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="16"/>
       <c r="D33" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="51"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="51"/>
+      <c r="B35" s="53"/>
       <c r="C35" s="6"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="50" t="s">
-        <v>136</v>
+      <c r="B36" s="52" t="s">
+        <v>128</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="50"/>
+      <c r="B37" s="52"/>
       <c r="C37" s="5"/>
       <c r="D37" s="1"/>
       <c r="F37" s="15"/>
     </row>
     <row r="38" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="51"/>
+      <c r="B38" s="53"/>
       <c r="C38" s="5"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="51"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="5"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="51"/>
+      <c r="B40" s="53"/>
       <c r="C40" s="6"/>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D41" s="70"/>
+      <c r="D41" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2071,40 +2096,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="53"/>
+      <c r="C3" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2115,59 +2140,59 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:6" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="57"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:6" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="57"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="57"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="50" t="s">
-        <v>110</v>
+      <c r="B12" s="52" t="s">
+        <v>108</v>
       </c>
       <c r="C12" s="46"/>
       <c r="D12" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="51"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="5"/>
       <c r="D13" s="45"/>
     </row>
     <row r="14" spans="2:6" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="51"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="44"/>
       <c r="D14" s="43"/>
     </row>
@@ -2206,40 +2231,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="53"/>
+      <c r="C3" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2250,82 +2275,82 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="55.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="57"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="57"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="57"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="57"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="50" t="s">
-        <v>113</v>
+      <c r="B13" s="52" t="s">
+        <v>111</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="51"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="51"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="2:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="50" t="s">
-        <v>114</v>
+      <c r="B16" s="52" t="s">
+        <v>112</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="51"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="5"/>
       <c r="D17" s="45"/>
     </row>
     <row r="18" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="51"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="44"/>
       <c r="D18" s="43"/>
     </row>
@@ -2349,7 +2374,7 @@
   <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2365,40 +2390,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2409,17 +2434,17 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="49" t="s">
-        <v>127</v>
+      <c r="D7" s="48" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="57"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2439,10 +2464,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C7ADAA-F745-434B-8977-383BAFA1EFD9}">
-  <dimension ref="B1:D13"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2458,40 +2483,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2502,53 +2527,38 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
+    <row r="8" spans="2:4" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="59"/>
       <c r="C8" s="10"/>
       <c r="D8" s="47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="57"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="57"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="45"/>
-    </row>
-    <row r="12" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="57"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="45"/>
-    </row>
-    <row r="13" spans="2:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="57"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="43"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="72"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="50"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B10:B13"/>
+  <mergeCells count="5">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -2590,10 +2600,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="63"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2601,10 +2611,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="61"/>
+      <c r="C3" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="63"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2612,10 +2622,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="61"/>
+      <c r="C4" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="63"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2623,15 +2633,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="59"/>
+      <c r="C5" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="61"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2644,59 +2654,59 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="63"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="63"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="23"/>
       <c r="D8" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="63"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="23"/>
       <c r="D9" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="63"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="62" t="s">
-        <v>36</v>
+      <c r="B11" s="64" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="63"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
-      <c r="B13" s="63"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="20"/>
       <c r="D13" s="19"/>
       <c r="E13" s="18"/>
@@ -2723,7 +2733,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2748,10 +2758,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="63"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2759,10 +2769,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="61"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2770,10 +2780,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="61"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2781,15 +2791,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="59"/>
+      <c r="C5" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="61"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -2802,103 +2812,103 @@
     </row>
     <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="63"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="63"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="63"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="63"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="63"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="63"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
-      <c r="B13" s="63"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="23"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
-      <c r="B15" s="63"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
-      <c r="B16" s="63"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="20"/>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
-      <c r="B17" s="62" t="s">
-        <v>75</v>
+      <c r="B17" s="64" t="s">
+        <v>74</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
-      <c r="B18" s="64"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="23"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
-      <c r="B19" s="64"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="36"/>
       <c r="D19" s="19"/>
       <c r="E19" s="18"/>
@@ -2925,7 +2935,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2950,10 +2960,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="63"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2961,10 +2971,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="61"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2972,10 +2982,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="61"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2983,15 +2993,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="59"/>
+      <c r="C5" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="61"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -3004,68 +3014,68 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="63"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="40"/>
       <c r="D7" s="39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="63"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="63"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="23"/>
       <c r="D9" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="63"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="63"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="62" t="s">
-        <v>83</v>
+      <c r="B12" s="64" t="s">
+        <v>82</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
-      <c r="B13" s="63"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="21"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="20"/>
       <c r="D14" s="19"/>
       <c r="E14" s="18"/>
@@ -3108,40 +3118,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3152,17 +3162,17 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="6"/>
       <c r="D8" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3201,40 +3211,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="53"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="55"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3245,49 +3255,49 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="59"/>
+      <c r="C8" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
-      <c r="C8" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="57"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="57"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="50" t="s">
-        <v>57</v>
+      <c r="B11" s="52" t="s">
+        <v>56</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="51"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="51"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
@@ -3328,40 +3338,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3372,49 +3382,49 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="57"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="57"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="57"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="50" t="s">
-        <v>90</v>
+      <c r="B11" s="52" t="s">
+        <v>88</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="51"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="51"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
@@ -3464,10 +3474,10 @@
       <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="63"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3475,10 +3485,10 @@
       <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="61"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3486,10 +3496,10 @@
       <c r="B4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="61"/>
+      <c r="C4" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="63"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3497,15 +3507,15 @@
       <c r="B5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="59"/>
+      <c r="C5" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="61"/>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="64" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -3518,165 +3528,165 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
-      <c r="B7" s="63"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
-      <c r="B8" s="63"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="23"/>
       <c r="D8" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="45.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
-      <c r="B9" s="63"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="23"/>
       <c r="D9" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
-      <c r="B10" s="63"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
-      <c r="B11" s="63"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="23"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
-      <c r="B12" s="63"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
-      <c r="B13" s="63"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="23"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
-      <c r="B15" s="63"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
-      <c r="B16" s="63"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="20"/>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
-      <c r="B17" s="62" t="s">
-        <v>66</v>
+      <c r="B17" s="64" t="s">
+        <v>65</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
-      <c r="B18" s="63"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="23"/>
       <c r="D18" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
-      <c r="B19" s="63"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="21"/>
-      <c r="B20" s="63"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="34"/>
       <c r="D20" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="21"/>
-      <c r="B21" s="63"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="34"/>
       <c r="D21" s="33"/>
       <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="21"/>
-      <c r="B22" s="63"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="20"/>
       <c r="D22" s="19"/>
       <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="62" t="s">
-        <v>62</v>
+      <c r="B23" s="64" t="s">
+        <v>61</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="63"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="23"/>
       <c r="D24" s="22"/>
     </row>
     <row r="25" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="63"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="34"/>
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="63"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="34"/>
       <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:5" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="63"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="34"/>
       <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="63"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="20"/>
       <c r="D28" s="19"/>
     </row>
@@ -3703,7 +3713,7 @@
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3719,40 +3729,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3763,24 +3773,24 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="57"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="57"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
foi bom enquanto durou, mas hoje acabou
</commit_message>
<xml_diff>
--- a/UseCaseLI4.xlsx
+++ b/UseCaseLI4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaon\Desktop\LI4\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854AD0B2-9788-40E4-A2CE-164AE3115D21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C221D764-42D2-4453-A603-7B459D18FE04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registar conta" sheetId="1" r:id="rId1"/>
@@ -102,13 +102,7 @@
 a informação</t>
   </si>
   <si>
-    <t>Alterar preferências</t>
-  </si>
-  <si>
     <t>3. Verifica que não há ambiguidade entre preferências escolhidas.</t>
-  </si>
-  <si>
-    <t>São alteradas as preferências relativas ao cliente no sistema</t>
   </si>
   <si>
     <t>1. Seleciona os ingredientes que mais aprecia</t>
@@ -546,6 +540,12 @@
   </si>
   <si>
     <t>Visualizar lista de ingredientes da ementa semanal</t>
+  </si>
+  <si>
+    <t>Gerir preferências</t>
+  </si>
+  <si>
+    <t>As alterações realizadas sobre as preferências são guardadas</t>
   </si>
 </sst>
 </file>
@@ -1677,13 +1677,13 @@
       <c r="B7" s="59"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="59"/>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="11"/>
     </row>
@@ -1691,14 +1691,14 @@
       <c r="B9" s="59"/>
       <c r="C9" s="10"/>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1710,11 +1710,11 @@
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="52" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -1729,11 +1729,11 @@
     </row>
     <row r="15" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1782,7 +1782,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -1800,7 +1800,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="55"/>
     </row>
@@ -1809,7 +1809,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -1828,13 +1828,13 @@
       <c r="B7" s="71"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1842,27 +1842,27 @@
       <c r="B9" s="71"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="71"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="71"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="71"/>
       <c r="C12" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1870,7 +1870,7 @@
       <c r="B13" s="71"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -1880,17 +1880,17 @@
     </row>
     <row r="15" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="52"/>
       <c r="C16" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1898,14 +1898,14 @@
       <c r="B17" s="53"/>
       <c r="C17" s="5"/>
       <c r="D17" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="53"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G18" s="15"/>
     </row>
@@ -1917,11 +1917,11 @@
     </row>
     <row r="20" spans="2:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="68" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G20" s="15"/>
     </row>
@@ -1951,10 +1951,10 @@
     </row>
     <row r="25" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="52" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1962,13 +1962,13 @@
       <c r="B26" s="52"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="53"/>
       <c r="C27" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1984,10 +1984,10 @@
     </row>
     <row r="30" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="52" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1995,27 +1995,27 @@
       <c r="B31" s="52"/>
       <c r="C31" s="5"/>
       <c r="D31" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="53"/>
       <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="53"/>
       <c r="C33" s="16"/>
       <c r="D33" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="53"/>
       <c r="C34" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D34" s="1"/>
     </row>
@@ -2026,11 +2026,11 @@
     </row>
     <row r="36" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="52" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -2097,7 +2097,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -2106,7 +2106,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D3" s="55"/>
     </row>
@@ -2115,7 +2115,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="55"/>
     </row>
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -2142,7 +2142,7 @@
     <row r="7" spans="2:6" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2150,13 +2150,13 @@
       <c r="B8" s="59"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="59"/>
       <c r="C9" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2164,26 +2164,26 @@
       <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="47" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C12" s="46"/>
       <c r="D12" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -2232,7 +2232,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -2241,7 +2241,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D3" s="55"/>
     </row>
@@ -2250,7 +2250,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="55"/>
     </row>
@@ -2259,7 +2259,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -2277,7 +2277,7 @@
     <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2285,20 +2285,20 @@
       <c r="B8" s="59"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="55.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="59"/>
       <c r="C10" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2306,23 +2306,23 @@
       <c r="B11" s="59"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="59"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -2337,11 +2337,11 @@
     </row>
     <row r="16" spans="2:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -2391,7 +2391,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -2418,7 +2418,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -2437,14 +2437,14 @@
       <c r="B7" s="59"/>
       <c r="C7" s="10"/>
       <c r="D7" s="48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="59"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2466,7 +2466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C7ADAA-F745-434B-8977-383BAFA1EFD9}">
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2484,7 +2484,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -2502,7 +2502,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="55"/>
     </row>
@@ -2511,7 +2511,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -2529,7 +2529,7 @@
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2537,21 +2537,21 @@
       <c r="B8" s="59"/>
       <c r="C8" s="10"/>
       <c r="D8" s="47" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="72"/>
       <c r="C9" s="10"/>
       <c r="D9" s="51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="50"/>
       <c r="C10" s="13"/>
       <c r="D10" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -2575,7 +2575,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2601,7 +2601,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="18"/>
@@ -2612,7 +2612,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="18"/>
@@ -2623,7 +2623,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="18"/>
@@ -2634,7 +2634,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="18"/>
@@ -2656,7 +2656,7 @@
       <c r="A7" s="21"/>
       <c r="B7" s="65"/>
       <c r="C7" s="28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="18"/>
@@ -2666,7 +2666,7 @@
       <c r="B8" s="65"/>
       <c r="C8" s="23"/>
       <c r="D8" s="26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="18"/>
     </row>
@@ -2675,7 +2675,7 @@
       <c r="B9" s="65"/>
       <c r="C9" s="23"/>
       <c r="D9" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="18"/>
     </row>
@@ -2689,11 +2689,11 @@
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
       <c r="B11" s="64" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="18"/>
     </row>
@@ -2759,7 +2759,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="18"/>
@@ -2792,7 +2792,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="18"/>
@@ -2814,7 +2814,7 @@
       <c r="A7" s="21"/>
       <c r="B7" s="65"/>
       <c r="C7" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="18"/>
@@ -2824,7 +2824,7 @@
       <c r="B8" s="65"/>
       <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8" s="18"/>
     </row>
@@ -2832,7 +2832,7 @@
       <c r="A9" s="21"/>
       <c r="B9" s="65"/>
       <c r="C9" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="18"/>
@@ -2842,7 +2842,7 @@
       <c r="B10" s="65"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="18"/>
     </row>
@@ -2891,10 +2891,10 @@
     <row r="17" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
       <c r="B17" s="64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="18"/>
@@ -2961,7 +2961,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="18"/>
@@ -2994,7 +2994,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="18"/>
@@ -3017,7 +3017,7 @@
       <c r="B7" s="65"/>
       <c r="C7" s="40"/>
       <c r="D7" s="39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" s="18"/>
     </row>
@@ -3026,7 +3026,7 @@
       <c r="B8" s="65"/>
       <c r="C8" s="38"/>
       <c r="D8" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" s="18"/>
     </row>
@@ -3035,7 +3035,7 @@
       <c r="B9" s="65"/>
       <c r="C9" s="23"/>
       <c r="D9" s="35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E9" s="18"/>
     </row>
@@ -3043,7 +3043,7 @@
       <c r="A10" s="21"/>
       <c r="B10" s="65"/>
       <c r="C10" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="18"/>
@@ -3058,11 +3058,11 @@
     <row r="12" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
       <c r="B12" s="64" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="18"/>
     </row>
@@ -3101,7 +3101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -3119,7 +3119,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -3137,7 +3137,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="55"/>
     </row>
@@ -3146,7 +3146,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -3164,7 +3164,7 @@
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -3172,7 +3172,7 @@
       <c r="B8" s="59"/>
       <c r="C8" s="6"/>
       <c r="D8" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3258,13 +3258,13 @@
       <c r="B7" s="59"/>
       <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="59"/>
       <c r="C8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" s="11"/>
     </row>
@@ -3272,23 +3272,23 @@
       <c r="B9" s="59"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="59"/>
       <c r="C10" s="5"/>
       <c r="D10" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="52" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -3322,7 +3322,7 @@
   <dimension ref="B1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3339,7 +3339,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>19</v>
+        <v>148</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -3366,7 +3366,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="D5" s="57"/>
     </row>
@@ -3384,7 +3384,7 @@
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -3399,7 +3399,7 @@
       <c r="B9" s="59"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3411,11 +3411,11 @@
     </row>
     <row r="11" spans="2:4" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -3475,7 +3475,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="18"/>
@@ -3497,7 +3497,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="18"/>
@@ -3508,7 +3508,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="18"/>
@@ -3530,7 +3530,7 @@
       <c r="A7" s="21"/>
       <c r="B7" s="65"/>
       <c r="C7" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="18"/>
@@ -3540,7 +3540,7 @@
       <c r="B8" s="65"/>
       <c r="C8" s="23"/>
       <c r="D8" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E8" s="18"/>
     </row>
@@ -3549,7 +3549,7 @@
       <c r="B9" s="65"/>
       <c r="C9" s="23"/>
       <c r="D9" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" s="18"/>
     </row>
@@ -3558,7 +3558,7 @@
       <c r="B10" s="65"/>
       <c r="C10" s="23"/>
       <c r="D10" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10" s="18"/>
     </row>
@@ -3607,11 +3607,11 @@
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
       <c r="B17" s="64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E17" s="18"/>
     </row>
@@ -3620,7 +3620,7 @@
       <c r="B18" s="65"/>
       <c r="C18" s="23"/>
       <c r="D18" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" s="18"/>
     </row>
@@ -3628,7 +3628,7 @@
       <c r="A19" s="21"/>
       <c r="B19" s="65"/>
       <c r="C19" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="18"/>
@@ -3638,7 +3638,7 @@
       <c r="B20" s="65"/>
       <c r="C20" s="34"/>
       <c r="D20" s="33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E20" s="18"/>
     </row>
@@ -3658,10 +3658,10 @@
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="64" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="24"/>
     </row>
@@ -3730,7 +3730,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D2" s="55"/>
     </row>
@@ -3748,7 +3748,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="55"/>
     </row>
@@ -3775,7 +3775,7 @@
     <row r="7" spans="2:4" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1"/>
     </row>

</xml_diff>